<commit_message>
still testing upper part
</commit_message>
<xml_diff>
--- a/Output_testing/R1_201907/Country/HKD/MN/KIRIBATI_201907_HKD_MN.xlsx
+++ b/Output_testing/R1_201907/Country/HKD/MN/KIRIBATI_201907_HKD_MN.xlsx
@@ -641,10 +641,10 @@
         </is>
       </c>
       <c r="B10" s="1" t="n">
-        <v>202</v>
+        <v>203</v>
       </c>
       <c r="C10" s="2" t="n">
-        <v>205</v>
+        <v>206</v>
       </c>
       <c r="D10" s="8" t="n">
         <v>0.042046</v>

</xml_diff>